<commit_message>
Images graphiques données tp2
</commit_message>
<xml_diff>
--- a/tp1/Report/Test_data.xlsx
+++ b/tp1/Report/Test_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\GIF-7104-TP1\tp1\Rapport\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\GIF-7104-TP1\tp1\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="8">
   <si>
     <t>Temps d'exécution</t>
   </si>
@@ -39,6 +39,15 @@
   </si>
   <si>
     <t>Efficacité</t>
+  </si>
+  <si>
+    <t>Threads</t>
+  </si>
+  <si>
+    <t>Nombre d'applications</t>
+  </si>
+  <si>
+    <t>Temps</t>
   </si>
 </sst>
 </file>
@@ -128,9 +137,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-CA" baseline="0"/>
-              <a:t>Efficacité, Crible d'Ératosthène multifilaire</a:t>
+              <a:t>Efficacité selon le nombre de threads </a:t>
             </a:r>
-            <a:endParaRPr lang="fr-CA"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -170,374 +178,10 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>1 000 000 000 nbrs</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Feuil1!$G$2:$G$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Feuil1!$I$2:$I$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0336619968040113</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.92975309930888539</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.88026562239311978</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.74484212601151767</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.60832757564471596</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1CF5-4525-A17C-20C527D51B41}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>500 000 000 nbrs</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Feuil1!$G$9:$G$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Feuil1!$I$9:$I$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0817095469588494</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.88319958767304563</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.86674602719945293</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.61849939167815715</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.52247781030525997</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1CF5-4525-A17C-20C527D51B41}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>333 333 333 nbrs</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Feuil1!$G$16:$G$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Feuil1!$I$16:$I$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0941977898251085</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.97154754395056697</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.89174647095086168</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.62422402591147863</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.52218043322622343</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-1CF5-4525-A17C-20C527D51B41}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>250 000 000 nbrs</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Feuil1!$G$23:$G$28</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Feuil1!$I$23:$I$28</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0923048084541331</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.9086034548632046</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.73547682304548689</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.69499095308382253</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.53445713782769688</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-1CF5-4525-A17C-20C527D51B41}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>200 000 000 nbrs</c:v>
+            <c:v>100</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -565,10 +209,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$G$30:$G$35</c:f>
+              <c:f>Feuil1!$L$34:$L$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -581,38 +225,26 @@
                 <c:pt idx="3">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$I$30:$I$35</c:f>
+              <c:f>Feuil1!$P$34:$P$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0920097569538412</c:v>
+                  <c:v>0.72576620445250728</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.92181286815086205</c:v>
+                  <c:v>0.5856404288828595</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.88466745907972644</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.70335216519274102</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5356223306839728</c:v>
+                  <c:v>0.49886083906264245</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -620,7 +252,256 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-1CF5-4525-A17C-20C527D51B41}"/>
+              <c16:uniqueId val="{00000004-ADD7-4585-AEB4-E781B4AA5A44}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>75</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$L$40:$L$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$P$40:$P$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.7059995921167288</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.56387527710538199</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.49099379082203631</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-ADD7-4585-AEB4-E781B4AA5A44}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>50</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$L$46:$L$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$P$46:$P$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.68950020575033111</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.57796021358114991</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.48187162636957354</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-ADD7-4585-AEB4-E781B4AA5A44}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>25</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$L$46:$L$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$P$52:$P$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.70834637698178893</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.53654968301111561</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.47095563278832692</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-ADD7-4585-AEB4-E781B4AA5A44}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -634,12 +515,475 @@
         </c:dLbls>
         <c:axId val="60103088"/>
         <c:axId val="60103744"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:v>100</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:multiLvlStrRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Feuil1!$L$37:$M$343</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:multiLvlStrCache>
+                      <c:ptCount val="19"/>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>100</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>Nombre d'applications</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>75</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>75</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>75</c:v>
+                        </c:pt>
+                        <c:pt idx="6">
+                          <c:v>75</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>Nombre d'applications</c:v>
+                        </c:pt>
+                        <c:pt idx="9">
+                          <c:v>50</c:v>
+                        </c:pt>
+                        <c:pt idx="10">
+                          <c:v>50</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
+                          <c:v>50</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>50</c:v>
+                        </c:pt>
+                        <c:pt idx="14">
+                          <c:v>Nombre d'applications</c:v>
+                        </c:pt>
+                        <c:pt idx="15">
+                          <c:v>25</c:v>
+                        </c:pt>
+                        <c:pt idx="16">
+                          <c:v>25</c:v>
+                        </c:pt>
+                        <c:pt idx="17">
+                          <c:v>25</c:v>
+                        </c:pt>
+                        <c:pt idx="18">
+                          <c:v>25</c:v>
+                        </c:pt>
+                      </c:lvl>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>4</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>Threads</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>1</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>2</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>3</c:v>
+                        </c:pt>
+                        <c:pt idx="6">
+                          <c:v>4</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>Threads</c:v>
+                        </c:pt>
+                        <c:pt idx="9">
+                          <c:v>1</c:v>
+                        </c:pt>
+                        <c:pt idx="10">
+                          <c:v>2</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
+                          <c:v>3</c:v>
+                        </c:pt>
+                        <c:pt idx="12">
+                          <c:v>4</c:v>
+                        </c:pt>
+                        <c:pt idx="14">
+                          <c:v>Threads</c:v>
+                        </c:pt>
+                        <c:pt idx="15">
+                          <c:v>1</c:v>
+                        </c:pt>
+                        <c:pt idx="16">
+                          <c:v>2</c:v>
+                        </c:pt>
+                        <c:pt idx="17">
+                          <c:v>3</c:v>
+                        </c:pt>
+                        <c:pt idx="18">
+                          <c:v>4</c:v>
+                        </c:pt>
+                      </c:lvl>
+                    </c:multiLvlStrCache>
+                  </c:multiLvlStrRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Feuil1!$O$34:$O$37</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.4515324089050146</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1.7569212866485784</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1.9954433562505698</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-ADD7-4585-AEB4-E781B4AA5A44}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:v>75</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Feuil1!$L$40:$L$43</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Feuil1!$O$40:$O$43</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.4119991842334576</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1.6916258313161459</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1.9639751632881453</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-ADD7-4585-AEB4-E781B4AA5A44}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:v>50</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Feuil1!$L$46:$L$49</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Feuil1!$O$46:$O$49</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.3790004115006622</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1.7338806407434497</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1.9274865054782941</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-ADD7-4585-AEB4-E781B4AA5A44}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:v>25</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Feuil1!$L$52:$L$55</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Feuil1!$O$52:$O$55</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="4"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.4166927539635779</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1.6096490490333468</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1.8838225311533077</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-ADD7-4585-AEB4-E781B4AA5A44}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="60103088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="6"/>
+          <c:max val="4"/>
           <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -683,7 +1027,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="fr-CA" baseline="0"/>
-                  <a:t> de fils</a:t>
+                  <a:t> de fils d'exécution</a:t>
                 </a:r>
                 <a:endParaRPr lang="fr-CA"/>
               </a:p>
@@ -765,6 +1109,8 @@
         <c:axId val="60103744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1515,15 +1861,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>171449</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:colOff>495299</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>104774</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>36194</xdr:rowOff>
+      <xdr:colOff>428624</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>55244</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1848,10 +2194,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
+      <selection activeCell="T30" sqref="T30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1861,6 +2207,7 @@
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1903,7 +2250,7 @@
         <v>16.777985999999999</v>
       </c>
       <c r="F2">
-        <v>1000000000</v>
+        <v>100</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -1931,7 +2278,7 @@
         <v>8.1157990000000009</v>
       </c>
       <c r="F3">
-        <v>1000000000</v>
+        <v>100</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -1959,7 +2306,7 @@
         <v>6.015212</v>
       </c>
       <c r="F4">
-        <v>1000000000</v>
+        <v>100</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -1987,7 +2334,7 @@
         <v>4.7650350000000001</v>
       </c>
       <c r="F5">
-        <v>1000000000</v>
+        <v>100</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -2015,7 +2362,7 @@
         <v>4.5051119999999996</v>
       </c>
       <c r="F6">
-        <v>1000000000</v>
+        <v>100</v>
       </c>
       <c r="G6">
         <v>5</v>
@@ -2043,7 +2390,7 @@
         <v>4.5967520000000004</v>
       </c>
       <c r="F7">
-        <v>1000000000</v>
+        <v>100</v>
       </c>
       <c r="G7">
         <v>6</v>
@@ -2097,7 +2444,7 @@
         <v>7.6254790000000003</v>
       </c>
       <c r="F9">
-        <v>500000000</v>
+        <v>100</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -2125,7 +2472,7 @@
         <v>3.5247350000000002</v>
       </c>
       <c r="F10">
-        <v>500000000</v>
+        <v>100</v>
       </c>
       <c r="G10">
         <v>2</v>
@@ -2153,7 +2500,7 @@
         <v>2.8779750000000002</v>
       </c>
       <c r="F11">
-        <v>500000000</v>
+        <v>100</v>
       </c>
       <c r="G11">
         <v>3</v>
@@ -2181,7 +2528,7 @@
         <v>2.1994560000000001</v>
       </c>
       <c r="F12">
-        <v>500000000</v>
+        <v>100</v>
       </c>
       <c r="G12">
         <v>4</v>
@@ -2209,7 +2556,7 @@
         <v>2.4658000000000002</v>
       </c>
       <c r="F13">
-        <v>500000000</v>
+        <v>100</v>
       </c>
       <c r="G13">
         <v>5</v>
@@ -2237,7 +2584,7 @@
         <v>2.4324729999999999</v>
       </c>
       <c r="F14">
-        <v>500000000</v>
+        <v>100</v>
       </c>
       <c r="G14">
         <v>6</v>
@@ -2291,7 +2638,7 @@
         <v>5.0224159999999998</v>
       </c>
       <c r="F16">
-        <v>333333333</v>
+        <v>100</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -2319,7 +2666,7 @@
         <v>2.2950219999999999</v>
       </c>
       <c r="F17">
-        <v>333333333</v>
+        <v>100</v>
       </c>
       <c r="G17">
         <v>2</v>
@@ -2347,7 +2694,7 @@
         <v>1.7231669999999999</v>
       </c>
       <c r="F18">
-        <v>333333333</v>
+        <v>100</v>
       </c>
       <c r="G18">
         <v>3</v>
@@ -2375,7 +2722,7 @@
         <v>1.4080280000000001</v>
       </c>
       <c r="F19">
-        <v>333333333</v>
+        <v>100</v>
       </c>
       <c r="G19">
         <v>4</v>
@@ -2403,7 +2750,7 @@
         <v>1.6091709999999999</v>
       </c>
       <c r="F20">
-        <v>333333333</v>
+        <v>100</v>
       </c>
       <c r="G20">
         <v>5</v>
@@ -2431,7 +2778,7 @@
         <v>1.603027</v>
       </c>
       <c r="F21">
-        <v>333333333</v>
+        <v>100</v>
       </c>
       <c r="G21">
         <v>6</v>
@@ -2485,7 +2832,7 @@
         <v>3.752694</v>
       </c>
       <c r="F23">
-        <v>250000000</v>
+        <v>100</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -2513,7 +2860,7 @@
         <v>1.717787</v>
       </c>
       <c r="F24">
-        <v>250000000</v>
+        <v>100</v>
       </c>
       <c r="G24">
         <v>2</v>
@@ -2541,7 +2888,7 @@
         <v>1.3767259999999999</v>
       </c>
       <c r="F25">
-        <v>250000000</v>
+        <v>100</v>
       </c>
       <c r="G25">
         <v>3</v>
@@ -2569,7 +2916,7 @@
         <v>1.2755989999999999</v>
       </c>
       <c r="F26">
-        <v>250000000</v>
+        <v>100</v>
       </c>
       <c r="G26">
         <v>4</v>
@@ -2588,7 +2935,7 @@
         <v>1.0799259999999999</v>
       </c>
       <c r="F27">
-        <v>250000000</v>
+        <v>100</v>
       </c>
       <c r="G27">
         <v>5</v>
@@ -2607,7 +2954,7 @@
         <v>1.1702509999999999</v>
       </c>
       <c r="F28">
-        <v>250000000</v>
+        <v>100</v>
       </c>
       <c r="G28">
         <v>6</v>
@@ -2643,7 +2990,7 @@
         <v>2.9860570000000002</v>
       </c>
       <c r="F30">
-        <v>200000000</v>
+        <v>100</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -2662,7 +3009,7 @@
         <v>1.3672299999999999</v>
       </c>
       <c r="F31">
-        <v>200000000</v>
+        <v>100</v>
       </c>
       <c r="G31">
         <v>2</v>
@@ -2681,7 +3028,7 @@
         <v>1.079777</v>
       </c>
       <c r="F32">
-        <v>200000000</v>
+        <v>100</v>
       </c>
       <c r="G32">
         <v>3</v>
@@ -2695,12 +3042,12 @@
         <v>0.92181286815086205</v>
       </c>
     </row>
-    <row r="33" spans="5:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E33">
         <v>0.84383600000000003</v>
       </c>
       <c r="F33">
-        <v>200000000</v>
+        <v>100</v>
       </c>
       <c r="G33">
         <v>4</v>
@@ -2713,13 +3060,28 @@
         <f t="shared" si="1"/>
         <v>0.88466745907972644</v>
       </c>
-    </row>
-    <row r="34" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="L33" t="s">
+        <v>5</v>
+      </c>
+      <c r="M33" t="s">
+        <v>6</v>
+      </c>
+      <c r="N33" t="s">
+        <v>7</v>
+      </c>
+      <c r="O33" t="s">
+        <v>3</v>
+      </c>
+      <c r="P33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E34">
         <v>0.84909299999999999</v>
       </c>
       <c r="F34">
-        <v>200000000</v>
+        <v>100</v>
       </c>
       <c r="G34">
         <v>5</v>
@@ -2732,10 +3094,30 @@
         <f t="shared" si="1"/>
         <v>0.70335216519274102</v>
       </c>
-    </row>
-    <row r="35" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <v>100</v>
+      </c>
+      <c r="N34">
+        <v>33.550767999999998</v>
+      </c>
+      <c r="O34">
+        <f>$N$34/N34</f>
+        <v>1</v>
+      </c>
+      <c r="P34">
+        <f>O34/L34</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E35">
         <v>0.92915499999999995</v>
+      </c>
+      <c r="F35">
+        <v>100</v>
       </c>
       <c r="G35">
         <v>6</v>
@@ -2747,6 +3129,340 @@
       <c r="I35">
         <f t="shared" si="1"/>
         <v>0.5356223306839728</v>
+      </c>
+      <c r="L35">
+        <v>2</v>
+      </c>
+      <c r="M35">
+        <v>100</v>
+      </c>
+      <c r="N35">
+        <v>23.114032999999999</v>
+      </c>
+      <c r="O35">
+        <f t="shared" ref="O35:O37" si="6">$N$34/N35</f>
+        <v>1.4515324089050146</v>
+      </c>
+      <c r="P35">
+        <f t="shared" ref="P35:P37" si="7">O35/L35</f>
+        <v>0.72576620445250728</v>
+      </c>
+    </row>
+    <row r="36" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="L36">
+        <v>3</v>
+      </c>
+      <c r="M36">
+        <v>100</v>
+      </c>
+      <c r="N36">
+        <v>19.096340999999999</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="6"/>
+        <v>1.7569212866485784</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="7"/>
+        <v>0.5856404288828595</v>
+      </c>
+    </row>
+    <row r="37" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="L37">
+        <v>4</v>
+      </c>
+      <c r="M37">
+        <v>100</v>
+      </c>
+      <c r="N37">
+        <v>16.813690999999999</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="6"/>
+        <v>1.9954433562505698</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="7"/>
+        <v>0.49886083906264245</v>
+      </c>
+    </row>
+    <row r="39" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="L39" t="s">
+        <v>5</v>
+      </c>
+      <c r="M39" t="s">
+        <v>6</v>
+      </c>
+      <c r="N39" t="s">
+        <v>7</v>
+      </c>
+      <c r="O39" t="s">
+        <v>3</v>
+      </c>
+      <c r="P39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="M40">
+        <v>75</v>
+      </c>
+      <c r="N40">
+        <v>25.89406</v>
+      </c>
+      <c r="O40">
+        <f>$N$40/N40</f>
+        <v>1</v>
+      </c>
+      <c r="P40">
+        <f>O40/L40</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="L41">
+        <v>2</v>
+      </c>
+      <c r="M41">
+        <v>75</v>
+      </c>
+      <c r="N41">
+        <v>18.33858</v>
+      </c>
+      <c r="O41">
+        <f t="shared" ref="O41:O43" si="8">$N$40/N41</f>
+        <v>1.4119991842334576</v>
+      </c>
+      <c r="P41">
+        <f t="shared" ref="P41:P43" si="9">O41/L41</f>
+        <v>0.7059995921167288</v>
+      </c>
+    </row>
+    <row r="42" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="L42">
+        <v>3</v>
+      </c>
+      <c r="M42">
+        <v>75</v>
+      </c>
+      <c r="N42">
+        <v>15.307202999999999</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="8"/>
+        <v>1.6916258313161459</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="9"/>
+        <v>0.56387527710538199</v>
+      </c>
+    </row>
+    <row r="43" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="L43">
+        <v>4</v>
+      </c>
+      <c r="M43">
+        <v>75</v>
+      </c>
+      <c r="N43">
+        <v>13.184514999999999</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="8"/>
+        <v>1.9639751632881453</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="9"/>
+        <v>0.49099379082203631</v>
+      </c>
+    </row>
+    <row r="45" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="L45" t="s">
+        <v>5</v>
+      </c>
+      <c r="M45" t="s">
+        <v>6</v>
+      </c>
+      <c r="N45" t="s">
+        <v>7</v>
+      </c>
+      <c r="O45" t="s">
+        <v>3</v>
+      </c>
+      <c r="P45" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="L46">
+        <v>1</v>
+      </c>
+      <c r="M46">
+        <v>50</v>
+      </c>
+      <c r="N46">
+        <v>16.943414000000001</v>
+      </c>
+      <c r="O46">
+        <f>$N$46/N46</f>
+        <v>1</v>
+      </c>
+      <c r="P46">
+        <f>O46/L46</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="L47">
+        <v>2</v>
+      </c>
+      <c r="M47">
+        <v>50</v>
+      </c>
+      <c r="N47">
+        <v>12.286735999999999</v>
+      </c>
+      <c r="O47">
+        <f t="shared" ref="O47:O49" si="10">$N$46/N47</f>
+        <v>1.3790004115006622</v>
+      </c>
+      <c r="P47">
+        <f t="shared" ref="P47:P49" si="11">O47/L47</f>
+        <v>0.68950020575033111</v>
+      </c>
+    </row>
+    <row r="48" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="L48">
+        <v>3</v>
+      </c>
+      <c r="M48">
+        <v>50</v>
+      </c>
+      <c r="N48">
+        <v>9.7719609999999992</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="10"/>
+        <v>1.7338806407434497</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="11"/>
+        <v>0.57796021358114991</v>
+      </c>
+    </row>
+    <row r="49" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L49">
+        <v>4</v>
+      </c>
+      <c r="M49">
+        <v>50</v>
+      </c>
+      <c r="N49">
+        <v>8.790419</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="10"/>
+        <v>1.9274865054782941</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="11"/>
+        <v>0.48187162636957354</v>
+      </c>
+    </row>
+    <row r="51" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L51" t="s">
+        <v>5</v>
+      </c>
+      <c r="M51" t="s">
+        <v>6</v>
+      </c>
+      <c r="N51" t="s">
+        <v>7</v>
+      </c>
+      <c r="O51" t="s">
+        <v>3</v>
+      </c>
+      <c r="P51" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L52">
+        <v>1</v>
+      </c>
+      <c r="M52">
+        <v>25</v>
+      </c>
+      <c r="N52">
+        <v>8.5169669999999993</v>
+      </c>
+      <c r="O52">
+        <f>$N$52/N52</f>
+        <v>1</v>
+      </c>
+      <c r="P52">
+        <f>O52/L52</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L53">
+        <v>2</v>
+      </c>
+      <c r="M53">
+        <v>25</v>
+      </c>
+      <c r="N53">
+        <v>6.0118660000000004</v>
+      </c>
+      <c r="O53">
+        <f t="shared" ref="O53:O55" si="12">$N$52/N53</f>
+        <v>1.4166927539635779</v>
+      </c>
+      <c r="P53">
+        <f t="shared" ref="P53:P55" si="13">O53/L53</f>
+        <v>0.70834637698178893</v>
+      </c>
+    </row>
+    <row r="54" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L54">
+        <v>3</v>
+      </c>
+      <c r="M54">
+        <v>25</v>
+      </c>
+      <c r="N54">
+        <v>5.2911950000000001</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="12"/>
+        <v>1.6096490490333468</v>
+      </c>
+      <c r="P54">
+        <f t="shared" si="13"/>
+        <v>0.53654968301111561</v>
+      </c>
+    </row>
+    <row r="55" spans="12:16" x14ac:dyDescent="0.25">
+      <c r="L55">
+        <v>4</v>
+      </c>
+      <c r="M55">
+        <v>25</v>
+      </c>
+      <c r="N55">
+        <v>4.521109</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="12"/>
+        <v>1.8838225311533077</v>
+      </c>
+      <c r="P55">
+        <f t="shared" si="13"/>
+        <v>0.47095563278832692</v>
       </c>
     </row>
   </sheetData>

</xml_diff>